<commit_message>
Changed Emin of Z = 23 and A = 47
</commit_message>
<xml_diff>
--- a/log_book_new.xlsx
+++ b/log_book_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/OhioUniversity/PhD/NLDD/data_sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/NLD_database_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B4CBFB-F9D9-B645-B6B3-C873E00822AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5746031E-33C6-A345-8833-71A1EC8B3F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -2450,9 +2450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E8AA59-B14F-2247-92C6-86B2A5AEEF23}">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L114" sqref="L114"/>
+      <selection pane="topRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3930,7 +3930,7 @@
         <v>47</v>
       </c>
       <c r="E33">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F33">
         <v>7</v>

</xml_diff>

<commit_message>
Removed a few filters from log book
</commit_message>
<xml_diff>
--- a/log_book_new.xlsx
+++ b/log_book_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/NLD_database_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5746031E-33C6-A345-8833-71A1EC8B3F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3670F703-2D12-C14E-B3E9-205D1501C262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
+    <workbookView xWindow="-200" yWindow="2340" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -2450,9 +2450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E8AA59-B14F-2247-92C6-86B2A5AEEF23}">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I40" sqref="I40"/>
+      <selection pane="topRight" activeCell="H266" sqref="H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Log book without filters
</commit_message>
<xml_diff>
--- a/log_book_new.xlsx
+++ b/log_book_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/NLD_database_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3670F703-2D12-C14E-B3E9-205D1501C262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F38E5C-0777-604F-BD30-20F44414EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="2340" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
+    <workbookView xWindow="0" yWindow="1300" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
Checked a few references before 52V
</commit_message>
<xml_diff>
--- a/log_book_new.xlsx
+++ b/log_book_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/NLD_database_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5579B16-8501-5E4A-ABE0-560B5573C2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD582FF-C53A-4647-90E4-5BD5B7315651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
   </bookViews>
@@ -2466,7 +2466,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L26" sqref="L26"/>
+      <selection pane="topRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a few more reactions and checked references
</commit_message>
<xml_diff>
--- a/log_book_new.xlsx
+++ b/log_book_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragrathi/Desktop/NLD_database_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD582FF-C53A-4647-90E4-5BD5B7315651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C47BC1-5E1B-3E4C-AC9A-56155F3C744D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19340" xr2:uid="{9DC6FD1D-072D-EA4D-8753-22EDA1FE1D9C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="652">
   <si>
     <t>Isotope</t>
   </si>
@@ -2466,7 +2466,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L13" sqref="L13"/>
+      <selection pane="topRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3802,6 +3802,9 @@
       <c r="H28" t="s">
         <v>13</v>
       </c>
+      <c r="I28" t="s">
+        <v>108</v>
+      </c>
       <c r="J28">
         <v>0.318</v>
       </c>
@@ -3809,7 +3812,7 @@
         <v>434</v>
       </c>
       <c r="L28" t="s">
-        <v>227</v>
+        <v>646</v>
       </c>
       <c r="M28"/>
       <c r="N28" t="s">
@@ -3995,6 +3998,9 @@
       <c r="H32" t="s">
         <v>500</v>
       </c>
+      <c r="I32" t="s">
+        <v>617</v>
+      </c>
       <c r="J32" t="s">
         <v>14</v>
       </c>
@@ -4334,6 +4340,9 @@
       <c r="H39" t="s">
         <v>13</v>
       </c>
+      <c r="I39" t="s">
+        <v>108</v>
+      </c>
       <c r="J39">
         <v>0.21199999999999999</v>
       </c>
@@ -4341,7 +4350,7 @@
         <v>434</v>
       </c>
       <c r="L39" t="s">
-        <v>227</v>
+        <v>646</v>
       </c>
       <c r="M39"/>
       <c r="N39" t="s">

</xml_diff>